<commit_message>
Added Cells Pivot Table methods
</commit_message>
<xml_diff>
--- a/Aspose.CloudTests/TestData/cells-sample.xlsx
+++ b/Aspose.CloudTests/TestData/cells-sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,21 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="TestName">Sheet1!$H$7:$K$15</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId8"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>S. No</t>
   </si>
@@ -94,11 +99,95 @@
   <si>
     <t>Students Result Card</t>
   </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>Sum of Amount</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Beans</t>
+  </si>
+  <si>
+    <t>Broccoli</t>
+  </si>
+  <si>
+    <t>Carrots</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -235,12 +324,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -289,6 +494,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -325,6 +550,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -552,11 +778,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1116956720"/>
-        <c:axId val="1116963792"/>
+        <c:axId val="789001984"/>
+        <c:axId val="789002528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1116956720"/>
+        <c:axId val="789001984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1116963792"/>
+        <c:crossAx val="789002528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -607,7 +833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1116963792"/>
+        <c:axId val="789002528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +884,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1116956720"/>
+        <c:crossAx val="789001984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1569,6 +1795,1874 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="41397.516500925929" createdVersion="1" refreshedVersion="4" recordCount="213">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:F214" sheet="Sheet1" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Order ID" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="213"/>
+    </cacheField>
+    <cacheField name="Product" numFmtId="0">
+      <sharedItems count="7">
+        <s v="Carrots"/>
+        <s v="Broccoli"/>
+        <s v="Banana"/>
+        <s v="Beans"/>
+        <s v="Orange"/>
+        <s v="Apple"/>
+        <s v="Mango"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Vegetables"/>
+        <s v="Fruit"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Amount" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="107" maxValue="9990"/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2012-01-06T00:00:00" maxDate="2012-12-31T00:00:00"/>
+    </cacheField>
+    <cacheField name="Country" numFmtId="0">
+      <sharedItems count="7">
+        <s v="United States"/>
+        <s v="United Kingdom"/>
+        <s v="Canada"/>
+        <s v="Germany"/>
+        <s v="Australia"/>
+        <s v="New Zealand"/>
+        <s v="France"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="213">
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4270"/>
+    <d v="2012-01-06T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8239"/>
+    <d v="2012-01-07T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="617"/>
+    <d v="2012-01-08T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8384"/>
+    <d v="2012-01-10T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2626"/>
+    <d v="2012-01-10T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3610"/>
+    <d v="2012-01-11T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="9062"/>
+    <d v="2012-01-11T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6906"/>
+    <d v="2012-01-16T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2417"/>
+    <d v="2012-01-16T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7431"/>
+    <d v="2012-01-16T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8250"/>
+    <d v="2012-01-16T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="7012"/>
+    <d v="2012-01-18T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1903"/>
+    <d v="2012-01-20T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2824"/>
+    <d v="2012-01-22T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="6946"/>
+    <d v="2012-01-24T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2320"/>
+    <d v="2012-01-27T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2116"/>
+    <d v="2012-01-28T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1135"/>
+    <d v="2012-01-30T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3595"/>
+    <d v="2012-01-30T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1161"/>
+    <d v="2012-02-02T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="2256"/>
+    <d v="2012-02-04T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1004"/>
+    <d v="2012-02-11T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3642"/>
+    <d v="2012-02-14T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4582"/>
+    <d v="2012-02-17T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3559"/>
+    <d v="2012-02-17T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5154"/>
+    <d v="2012-02-17T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="7388"/>
+    <d v="2012-02-18T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="7163"/>
+    <d v="2012-02-18T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="5101"/>
+    <d v="2012-02-20T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7602"/>
+    <d v="2012-02-21T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="1641"/>
+    <d v="2012-02-22T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="8892"/>
+    <d v="2012-02-23T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2060"/>
+    <d v="2012-02-29T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1557"/>
+    <d v="2012-02-29T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="6509"/>
+    <d v="2012-03-01T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="5718"/>
+    <d v="2012-03-04T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7655"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9116"/>
+    <d v="2012-03-05T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2795"/>
+    <d v="2012-03-15T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5084"/>
+    <d v="2012-03-15T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="8941"/>
+    <d v="2012-03-15T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="5341"/>
+    <d v="2012-03-16T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="135"/>
+    <d v="2012-03-19T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="9400"/>
+    <d v="2012-03-19T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="6045"/>
+    <d v="2012-03-21T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="5820"/>
+    <d v="2012-03-22T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="8887"/>
+    <d v="2012-03-23T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="6982"/>
+    <d v="2012-03-24T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4029"/>
+    <d v="2012-03-26T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3665"/>
+    <d v="2012-03-26T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4781"/>
+    <d v="2012-03-29T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="52"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="3663"/>
+    <d v="2012-03-30T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="53"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="6331"/>
+    <d v="2012-04-01T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="54"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="4364"/>
+    <d v="2012-04-01T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="55"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="607"/>
+    <d v="2012-04-03T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="56"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1054"/>
+    <d v="2012-04-06T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7659"/>
+    <d v="2012-04-06T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="277"/>
+    <d v="2012-04-12T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="59"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="235"/>
+    <d v="2012-04-17T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="60"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1113"/>
+    <d v="2012-04-18T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1128"/>
+    <d v="2012-04-21T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="9231"/>
+    <d v="2012-04-22T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="63"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4387"/>
+    <d v="2012-04-23T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="64"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2763"/>
+    <d v="2012-04-25T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="65"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7898"/>
+    <d v="2012-04-27T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="66"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2427"/>
+    <d v="2012-04-30T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="67"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8663"/>
+    <d v="2012-05-01T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="68"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2789"/>
+    <d v="2012-05-01T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="69"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4054"/>
+    <d v="2012-05-02T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="70"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="2262"/>
+    <d v="2012-05-02T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="5600"/>
+    <d v="2012-05-02T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="72"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5787"/>
+    <d v="2012-05-03T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="73"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="6295"/>
+    <d v="2012-05-03T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="74"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="474"/>
+    <d v="2012-05-05T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="75"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="4325"/>
+    <d v="2012-05-05T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="76"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="592"/>
+    <d v="2012-05-06T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4330"/>
+    <d v="2012-05-08T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="78"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="9405"/>
+    <d v="2012-05-08T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="79"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7671"/>
+    <d v="2012-05-08T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5791"/>
+    <d v="2012-05-08T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="81"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6007"/>
+    <d v="2012-05-12T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="82"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5030"/>
+    <d v="2012-05-14T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="83"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6763"/>
+    <d v="2012-05-14T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="84"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4248"/>
+    <d v="2012-05-15T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="85"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="9543"/>
+    <d v="2012-05-16T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="86"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2054"/>
+    <d v="2012-05-16T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="87"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="7094"/>
+    <d v="2012-05-16T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="88"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6087"/>
+    <d v="2012-05-18T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="89"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="4264"/>
+    <d v="2012-05-19T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="90"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="9333"/>
+    <d v="2012-05-20T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="8775"/>
+    <d v="2012-05-22T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="92"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2011"/>
+    <d v="2012-05-23T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="93"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5632"/>
+    <d v="2012-05-25T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4904"/>
+    <d v="2012-05-25T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="95"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1002"/>
+    <d v="2012-05-25T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="96"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="8141"/>
+    <d v="2012-05-26T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="97"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3644"/>
+    <d v="2012-05-26T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1380"/>
+    <d v="2012-05-26T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8354"/>
+    <d v="2012-05-26T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="100"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5182"/>
+    <d v="2012-05-27T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="101"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2193"/>
+    <d v="2012-05-27T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="102"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="3647"/>
+    <d v="2012-05-28T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="103"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="4104"/>
+    <d v="2012-05-28T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="104"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7457"/>
+    <d v="2012-05-28T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="105"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="3767"/>
+    <d v="2012-05-29T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="106"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4685"/>
+    <d v="2012-05-30T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="107"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3917"/>
+    <d v="2012-06-04T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="108"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="521"/>
+    <d v="2012-06-04T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="109"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="5605"/>
+    <d v="2012-06-10T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="110"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="9630"/>
+    <d v="2012-06-11T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="111"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6941"/>
+    <d v="2012-06-20T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="112"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="7231"/>
+    <d v="2012-06-20T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="113"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8891"/>
+    <d v="2012-06-23T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="114"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="107"/>
+    <d v="2012-06-25T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="115"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4243"/>
+    <d v="2012-06-26T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="116"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4514"/>
+    <d v="2012-06-27T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="117"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="5480"/>
+    <d v="2012-07-02T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="118"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5002"/>
+    <d v="2012-07-02T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="119"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8530"/>
+    <d v="2012-07-05T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="120"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4819"/>
+    <d v="2012-07-07T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="121"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="6343"/>
+    <d v="2012-07-11T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="122"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="2318"/>
+    <d v="2012-07-13T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="123"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="220"/>
+    <d v="2012-07-20T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="124"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="6341"/>
+    <d v="2012-07-20T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="125"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="330"/>
+    <d v="2012-07-20T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="126"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3027"/>
+    <d v="2012-07-20T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="127"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="850"/>
+    <d v="2012-07-22T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="128"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8986"/>
+    <d v="2012-07-23T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="129"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3800"/>
+    <d v="2012-07-25T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="130"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5751"/>
+    <d v="2012-07-28T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="131"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1704"/>
+    <d v="2012-07-29T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="132"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7966"/>
+    <d v="2012-07-30T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="133"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="852"/>
+    <d v="2012-07-31T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="134"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="8416"/>
+    <d v="2012-07-31T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="135"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7144"/>
+    <d v="2012-08-01T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="136"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="7854"/>
+    <d v="2012-08-01T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="137"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="859"/>
+    <d v="2012-08-03T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="138"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8049"/>
+    <d v="2012-08-12T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="139"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2836"/>
+    <d v="2012-08-13T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="140"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1743"/>
+    <d v="2012-08-19T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="141"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="3844"/>
+    <d v="2012-08-23T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="142"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7490"/>
+    <d v="2012-08-24T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="143"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4483"/>
+    <d v="2012-08-25T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="144"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7333"/>
+    <d v="2012-08-27T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="145"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7654"/>
+    <d v="2012-08-28T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="146"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="3944"/>
+    <d v="2012-08-29T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="147"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="5761"/>
+    <d v="2012-08-29T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="148"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6864"/>
+    <d v="2012-09-01T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="149"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4016"/>
+    <d v="2012-09-01T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="150"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1841"/>
+    <d v="2012-09-02T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="151"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="424"/>
+    <d v="2012-09-05T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="152"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8765"/>
+    <d v="2012-09-07T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="153"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5583"/>
+    <d v="2012-09-08T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="154"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4390"/>
+    <d v="2012-09-09T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="155"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="352"/>
+    <d v="2012-09-09T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="156"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="8489"/>
+    <d v="2012-09-11T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="157"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7090"/>
+    <d v="2012-09-11T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="158"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7880"/>
+    <d v="2012-09-15T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="159"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3861"/>
+    <d v="2012-09-18T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="160"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="7927"/>
+    <d v="2012-09-19T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="161"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6162"/>
+    <d v="2012-09-20T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="162"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="5523"/>
+    <d v="2012-09-25T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="163"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="5936"/>
+    <d v="2012-09-25T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="164"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7251"/>
+    <d v="2012-09-26T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="165"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="6187"/>
+    <d v="2012-09-27T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="166"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3210"/>
+    <d v="2012-09-29T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="167"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="682"/>
+    <d v="2012-09-29T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="168"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="793"/>
+    <d v="2012-10-03T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="169"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5346"/>
+    <d v="2012-10-04T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="170"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7103"/>
+    <d v="2012-10-07T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="171"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4603"/>
+    <d v="2012-10-10T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="172"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="8160"/>
+    <d v="2012-10-16T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="173"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7171"/>
+    <d v="2012-10-23T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="174"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3552"/>
+    <d v="2012-10-23T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="175"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7273"/>
+    <d v="2012-10-25T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="176"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2402"/>
+    <d v="2012-10-26T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="177"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1197"/>
+    <d v="2012-10-26T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="178"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="5015"/>
+    <d v="2012-10-26T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="179"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="5818"/>
+    <d v="2012-11-02T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="180"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4399"/>
+    <d v="2012-11-03T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="181"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3011"/>
+    <d v="2012-11-03T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="182"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="4715"/>
+    <d v="2012-11-09T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="183"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="5321"/>
+    <d v="2012-11-12T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="184"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8894"/>
+    <d v="2012-11-15T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="185"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4846"/>
+    <d v="2012-11-25T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="186"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="284"/>
+    <d v="2012-11-25T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="187"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="8283"/>
+    <d v="2012-11-26T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="188"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="9990"/>
+    <d v="2012-11-28T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="189"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="9014"/>
+    <d v="2012-11-28T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="190"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1942"/>
+    <d v="2012-11-29T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="191"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="7223"/>
+    <d v="2012-11-30T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="192"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4673"/>
+    <d v="2012-12-02T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="193"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9104"/>
+    <d v="2012-12-04T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="194"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="6078"/>
+    <d v="2012-12-05T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="195"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3278"/>
+    <d v="2012-12-06T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="196"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="136"/>
+    <d v="2012-12-12T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="197"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8377"/>
+    <d v="2012-12-12T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="198"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2382"/>
+    <d v="2012-12-12T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="199"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8702"/>
+    <d v="2012-12-15T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="200"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5021"/>
+    <d v="2012-12-16T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="201"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1760"/>
+    <d v="2012-12-16T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="202"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4766"/>
+    <d v="2012-12-18T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="203"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1541"/>
+    <d v="2012-12-19T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="204"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="2782"/>
+    <d v="2012-12-20T00:00:00"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="205"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2455"/>
+    <d v="2012-12-20T00:00:00"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="206"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="4512"/>
+    <d v="2012-12-22T00:00:00"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="207"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="8752"/>
+    <d v="2012-12-22T00:00:00"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="208"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9127"/>
+    <d v="2012-12-25T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="209"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1777"/>
+    <d v="2012-12-28T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="210"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="680"/>
+    <d v="2012-12-28T00:00:00"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="211"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="958"/>
+    <d v="2012-12-29T00:00:00"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="212"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2613"/>
+    <d v="2012-12-29T00:00:00"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="213"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="339"/>
+    <d v="2012-12-30T00:00:00"/>
+    <x v="4"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="4" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+  <location ref="A3:I12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField axis="axisCol" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="8">
+        <item x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" numFmtId="14" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="8">
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="2" hier="0"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1871,11 +3965,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2230,7 +4324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -2292,4 +4386,1029 @@
     </mc:AlternateContent>
   </oleObjects>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" customWidth="1"/>
+    <col min="257" max="257" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="10.140625" customWidth="1"/>
+    <col min="259" max="259" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="8" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="7" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="11.140625" customWidth="1"/>
+    <col min="266" max="266" width="2.42578125" customWidth="1"/>
+    <col min="513" max="513" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="10.140625" customWidth="1"/>
+    <col min="515" max="515" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="516" max="516" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="517" max="517" width="8" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="7" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="521" max="521" width="11.140625" customWidth="1"/>
+    <col min="522" max="522" width="2.42578125" customWidth="1"/>
+    <col min="769" max="769" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="10.140625" customWidth="1"/>
+    <col min="771" max="771" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="772" max="772" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="773" max="773" width="8" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="775" max="775" width="7" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="777" max="777" width="11.140625" customWidth="1"/>
+    <col min="778" max="778" width="2.42578125" customWidth="1"/>
+    <col min="1025" max="1025" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="10.140625" customWidth="1"/>
+    <col min="1027" max="1027" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1028" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1029" max="1029" width="8" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1031" max="1031" width="7" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1033" max="1033" width="11.140625" customWidth="1"/>
+    <col min="1034" max="1034" width="2.42578125" customWidth="1"/>
+    <col min="1281" max="1281" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="10.140625" customWidth="1"/>
+    <col min="1283" max="1283" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1284" max="1284" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1285" max="1285" width="8" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1287" max="1287" width="7" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1289" max="1289" width="11.140625" customWidth="1"/>
+    <col min="1290" max="1290" width="2.42578125" customWidth="1"/>
+    <col min="1537" max="1537" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="10.140625" customWidth="1"/>
+    <col min="1539" max="1539" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1540" max="1540" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1541" max="1541" width="8" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1543" max="1543" width="7" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1545" max="1545" width="11.140625" customWidth="1"/>
+    <col min="1546" max="1546" width="2.42578125" customWidth="1"/>
+    <col min="1793" max="1793" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="10.140625" customWidth="1"/>
+    <col min="1795" max="1795" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1796" max="1796" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1797" max="1797" width="8" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1799" max="1799" width="7" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1801" max="1801" width="11.140625" customWidth="1"/>
+    <col min="1802" max="1802" width="2.42578125" customWidth="1"/>
+    <col min="2049" max="2049" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="10.140625" customWidth="1"/>
+    <col min="2051" max="2051" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2052" max="2052" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2053" max="2053" width="8" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2055" width="7" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2057" max="2057" width="11.140625" customWidth="1"/>
+    <col min="2058" max="2058" width="2.42578125" customWidth="1"/>
+    <col min="2305" max="2305" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="10.140625" customWidth="1"/>
+    <col min="2307" max="2307" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2308" max="2308" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2309" max="2309" width="8" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2311" max="2311" width="7" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2313" max="2313" width="11.140625" customWidth="1"/>
+    <col min="2314" max="2314" width="2.42578125" customWidth="1"/>
+    <col min="2561" max="2561" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="10.140625" customWidth="1"/>
+    <col min="2563" max="2563" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2564" max="2564" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2565" max="2565" width="8" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2567" max="2567" width="7" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2569" max="2569" width="11.140625" customWidth="1"/>
+    <col min="2570" max="2570" width="2.42578125" customWidth="1"/>
+    <col min="2817" max="2817" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="10.140625" customWidth="1"/>
+    <col min="2819" max="2819" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2820" max="2820" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2821" max="2821" width="8" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2823" max="2823" width="7" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2825" max="2825" width="11.140625" customWidth="1"/>
+    <col min="2826" max="2826" width="2.42578125" customWidth="1"/>
+    <col min="3073" max="3073" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="10.140625" customWidth="1"/>
+    <col min="3075" max="3075" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3076" max="3076" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3077" max="3077" width="8" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3079" max="3079" width="7" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3081" max="3081" width="11.140625" customWidth="1"/>
+    <col min="3082" max="3082" width="2.42578125" customWidth="1"/>
+    <col min="3329" max="3329" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="10.140625" customWidth="1"/>
+    <col min="3331" max="3331" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3332" max="3332" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3333" max="3333" width="8" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3335" width="7" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3337" max="3337" width="11.140625" customWidth="1"/>
+    <col min="3338" max="3338" width="2.42578125" customWidth="1"/>
+    <col min="3585" max="3585" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="10.140625" customWidth="1"/>
+    <col min="3587" max="3587" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3588" max="3588" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3589" max="3589" width="8" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3591" max="3591" width="7" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3593" max="3593" width="11.140625" customWidth="1"/>
+    <col min="3594" max="3594" width="2.42578125" customWidth="1"/>
+    <col min="3841" max="3841" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="10.140625" customWidth="1"/>
+    <col min="3843" max="3843" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3844" max="3844" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3845" max="3845" width="8" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3847" max="3847" width="7" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3849" max="3849" width="11.140625" customWidth="1"/>
+    <col min="3850" max="3850" width="2.42578125" customWidth="1"/>
+    <col min="4097" max="4097" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="10.140625" customWidth="1"/>
+    <col min="4099" max="4099" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4100" max="4100" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4101" max="4101" width="8" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4103" max="4103" width="7" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4105" max="4105" width="11.140625" customWidth="1"/>
+    <col min="4106" max="4106" width="2.42578125" customWidth="1"/>
+    <col min="4353" max="4353" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="10.140625" customWidth="1"/>
+    <col min="4355" max="4355" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4356" max="4356" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4357" max="4357" width="8" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4359" max="4359" width="7" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4361" max="4361" width="11.140625" customWidth="1"/>
+    <col min="4362" max="4362" width="2.42578125" customWidth="1"/>
+    <col min="4609" max="4609" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="10.140625" customWidth="1"/>
+    <col min="4611" max="4611" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4612" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4613" max="4613" width="8" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4615" max="4615" width="7" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4617" max="4617" width="11.140625" customWidth="1"/>
+    <col min="4618" max="4618" width="2.42578125" customWidth="1"/>
+    <col min="4865" max="4865" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="10.140625" customWidth="1"/>
+    <col min="4867" max="4867" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4868" max="4868" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4869" max="4869" width="8" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4871" max="4871" width="7" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4873" max="4873" width="11.140625" customWidth="1"/>
+    <col min="4874" max="4874" width="2.42578125" customWidth="1"/>
+    <col min="5121" max="5121" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="10.140625" customWidth="1"/>
+    <col min="5123" max="5123" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5124" max="5124" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5125" max="5125" width="8" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5127" max="5127" width="7" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5129" max="5129" width="11.140625" customWidth="1"/>
+    <col min="5130" max="5130" width="2.42578125" customWidth="1"/>
+    <col min="5377" max="5377" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="10.140625" customWidth="1"/>
+    <col min="5379" max="5379" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5380" max="5380" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5381" max="5381" width="8" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5383" max="5383" width="7" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5385" max="5385" width="11.140625" customWidth="1"/>
+    <col min="5386" max="5386" width="2.42578125" customWidth="1"/>
+    <col min="5633" max="5633" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="10.140625" customWidth="1"/>
+    <col min="5635" max="5635" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5636" max="5636" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5637" max="5637" width="8" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5639" max="5639" width="7" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5641" max="5641" width="11.140625" customWidth="1"/>
+    <col min="5642" max="5642" width="2.42578125" customWidth="1"/>
+    <col min="5889" max="5889" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="10.140625" customWidth="1"/>
+    <col min="5891" max="5891" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5892" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5893" max="5893" width="8" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5895" max="5895" width="7" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5897" max="5897" width="11.140625" customWidth="1"/>
+    <col min="5898" max="5898" width="2.42578125" customWidth="1"/>
+    <col min="6145" max="6145" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="10.140625" customWidth="1"/>
+    <col min="6147" max="6147" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6148" max="6148" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6149" max="6149" width="8" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6151" max="6151" width="7" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6153" max="6153" width="11.140625" customWidth="1"/>
+    <col min="6154" max="6154" width="2.42578125" customWidth="1"/>
+    <col min="6401" max="6401" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="10.140625" customWidth="1"/>
+    <col min="6403" max="6403" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6404" max="6404" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6405" max="6405" width="8" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6407" width="7" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6409" max="6409" width="11.140625" customWidth="1"/>
+    <col min="6410" max="6410" width="2.42578125" customWidth="1"/>
+    <col min="6657" max="6657" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="10.140625" customWidth="1"/>
+    <col min="6659" max="6659" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6660" max="6660" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6661" max="6661" width="8" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6663" max="6663" width="7" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6665" max="6665" width="11.140625" customWidth="1"/>
+    <col min="6666" max="6666" width="2.42578125" customWidth="1"/>
+    <col min="6913" max="6913" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="10.140625" customWidth="1"/>
+    <col min="6915" max="6915" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6916" max="6916" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6917" max="6917" width="8" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6919" max="6919" width="7" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6921" max="6921" width="11.140625" customWidth="1"/>
+    <col min="6922" max="6922" width="2.42578125" customWidth="1"/>
+    <col min="7169" max="7169" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="10.140625" customWidth="1"/>
+    <col min="7171" max="7171" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7172" max="7172" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7173" max="7173" width="8" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7175" max="7175" width="7" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7177" max="7177" width="11.140625" customWidth="1"/>
+    <col min="7178" max="7178" width="2.42578125" customWidth="1"/>
+    <col min="7425" max="7425" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="10.140625" customWidth="1"/>
+    <col min="7427" max="7427" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7428" max="7428" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7429" max="7429" width="8" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7431" max="7431" width="7" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7433" max="7433" width="11.140625" customWidth="1"/>
+    <col min="7434" max="7434" width="2.42578125" customWidth="1"/>
+    <col min="7681" max="7681" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="10.140625" customWidth="1"/>
+    <col min="7683" max="7683" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7684" max="7684" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7685" max="7685" width="8" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7687" width="7" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7689" max="7689" width="11.140625" customWidth="1"/>
+    <col min="7690" max="7690" width="2.42578125" customWidth="1"/>
+    <col min="7937" max="7937" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="10.140625" customWidth="1"/>
+    <col min="7939" max="7939" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7940" max="7940" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7941" max="7941" width="8" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7943" max="7943" width="7" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7945" max="7945" width="11.140625" customWidth="1"/>
+    <col min="7946" max="7946" width="2.42578125" customWidth="1"/>
+    <col min="8193" max="8193" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="10.140625" customWidth="1"/>
+    <col min="8195" max="8195" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8196" max="8196" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8197" max="8197" width="8" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8199" max="8199" width="7" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8201" max="8201" width="11.140625" customWidth="1"/>
+    <col min="8202" max="8202" width="2.42578125" customWidth="1"/>
+    <col min="8449" max="8449" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="10.140625" customWidth="1"/>
+    <col min="8451" max="8451" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8452" max="8452" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8453" max="8453" width="8" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8455" max="8455" width="7" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8457" max="8457" width="11.140625" customWidth="1"/>
+    <col min="8458" max="8458" width="2.42578125" customWidth="1"/>
+    <col min="8705" max="8705" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="10.140625" customWidth="1"/>
+    <col min="8707" max="8707" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8708" max="8708" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8709" max="8709" width="8" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8711" max="8711" width="7" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8713" max="8713" width="11.140625" customWidth="1"/>
+    <col min="8714" max="8714" width="2.42578125" customWidth="1"/>
+    <col min="8961" max="8961" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="10.140625" customWidth="1"/>
+    <col min="8963" max="8963" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8964" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8965" max="8965" width="8" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8967" max="8967" width="7" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8969" max="8969" width="11.140625" customWidth="1"/>
+    <col min="8970" max="8970" width="2.42578125" customWidth="1"/>
+    <col min="9217" max="9217" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="10.140625" customWidth="1"/>
+    <col min="9219" max="9219" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9220" max="9220" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9221" max="9221" width="8" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9223" max="9223" width="7" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9225" max="9225" width="11.140625" customWidth="1"/>
+    <col min="9226" max="9226" width="2.42578125" customWidth="1"/>
+    <col min="9473" max="9473" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="10.140625" customWidth="1"/>
+    <col min="9475" max="9475" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9476" max="9476" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9477" max="9477" width="8" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9479" max="9479" width="7" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9481" max="9481" width="11.140625" customWidth="1"/>
+    <col min="9482" max="9482" width="2.42578125" customWidth="1"/>
+    <col min="9729" max="9729" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="10.140625" customWidth="1"/>
+    <col min="9731" max="9731" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9732" max="9732" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9733" max="9733" width="8" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9735" max="9735" width="7" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9737" max="9737" width="11.140625" customWidth="1"/>
+    <col min="9738" max="9738" width="2.42578125" customWidth="1"/>
+    <col min="9985" max="9985" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="10.140625" customWidth="1"/>
+    <col min="9987" max="9987" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9988" max="9988" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9989" max="9989" width="8" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9991" max="9991" width="7" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9993" max="9993" width="11.140625" customWidth="1"/>
+    <col min="9994" max="9994" width="2.42578125" customWidth="1"/>
+    <col min="10241" max="10241" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="10.140625" customWidth="1"/>
+    <col min="10243" max="10243" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10244" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10245" max="10245" width="8" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10247" max="10247" width="7" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10249" max="10249" width="11.140625" customWidth="1"/>
+    <col min="10250" max="10250" width="2.42578125" customWidth="1"/>
+    <col min="10497" max="10497" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="10.140625" customWidth="1"/>
+    <col min="10499" max="10499" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10500" max="10500" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10501" max="10501" width="8" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10503" max="10503" width="7" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10505" max="10505" width="11.140625" customWidth="1"/>
+    <col min="10506" max="10506" width="2.42578125" customWidth="1"/>
+    <col min="10753" max="10753" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="10.140625" customWidth="1"/>
+    <col min="10755" max="10755" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10756" max="10756" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10757" max="10757" width="8" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10759" max="10759" width="7" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10761" max="10761" width="11.140625" customWidth="1"/>
+    <col min="10762" max="10762" width="2.42578125" customWidth="1"/>
+    <col min="11009" max="11009" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="10.140625" customWidth="1"/>
+    <col min="11011" max="11011" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11012" max="11012" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11013" max="11013" width="8" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11015" max="11015" width="7" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11017" max="11017" width="11.140625" customWidth="1"/>
+    <col min="11018" max="11018" width="2.42578125" customWidth="1"/>
+    <col min="11265" max="11265" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="10.140625" customWidth="1"/>
+    <col min="11267" max="11267" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11268" max="11268" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11269" max="11269" width="8" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11271" max="11271" width="7" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11273" max="11273" width="11.140625" customWidth="1"/>
+    <col min="11274" max="11274" width="2.42578125" customWidth="1"/>
+    <col min="11521" max="11521" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="10.140625" customWidth="1"/>
+    <col min="11523" max="11523" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11524" max="11524" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11525" max="11525" width="8" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11527" max="11527" width="7" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11529" max="11529" width="11.140625" customWidth="1"/>
+    <col min="11530" max="11530" width="2.42578125" customWidth="1"/>
+    <col min="11777" max="11777" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="10.140625" customWidth="1"/>
+    <col min="11779" max="11779" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11780" max="11780" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11781" max="11781" width="8" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11783" max="11783" width="7" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11785" max="11785" width="11.140625" customWidth="1"/>
+    <col min="11786" max="11786" width="2.42578125" customWidth="1"/>
+    <col min="12033" max="12033" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="10.140625" customWidth="1"/>
+    <col min="12035" max="12035" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12036" max="12036" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12037" max="12037" width="8" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12039" width="7" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12041" max="12041" width="11.140625" customWidth="1"/>
+    <col min="12042" max="12042" width="2.42578125" customWidth="1"/>
+    <col min="12289" max="12289" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="10.140625" customWidth="1"/>
+    <col min="12291" max="12291" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12292" max="12292" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12293" max="12293" width="8" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12295" max="12295" width="7" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12297" max="12297" width="11.140625" customWidth="1"/>
+    <col min="12298" max="12298" width="2.42578125" customWidth="1"/>
+    <col min="12545" max="12545" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="10.140625" customWidth="1"/>
+    <col min="12547" max="12547" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12548" max="12548" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12549" max="12549" width="8" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12551" max="12551" width="7" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12553" max="12553" width="11.140625" customWidth="1"/>
+    <col min="12554" max="12554" width="2.42578125" customWidth="1"/>
+    <col min="12801" max="12801" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="10.140625" customWidth="1"/>
+    <col min="12803" max="12803" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12804" max="12804" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="12805" max="12805" width="8" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12807" max="12807" width="7" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12809" max="12809" width="11.140625" customWidth="1"/>
+    <col min="12810" max="12810" width="2.42578125" customWidth="1"/>
+    <col min="13057" max="13057" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="10.140625" customWidth="1"/>
+    <col min="13059" max="13059" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13060" max="13060" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13061" max="13061" width="8" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13063" max="13063" width="7" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13065" max="13065" width="11.140625" customWidth="1"/>
+    <col min="13066" max="13066" width="2.42578125" customWidth="1"/>
+    <col min="13313" max="13313" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="10.140625" customWidth="1"/>
+    <col min="13315" max="13315" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13316" max="13316" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13317" max="13317" width="8" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13319" max="13319" width="7" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13321" max="13321" width="11.140625" customWidth="1"/>
+    <col min="13322" max="13322" width="2.42578125" customWidth="1"/>
+    <col min="13569" max="13569" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="10.140625" customWidth="1"/>
+    <col min="13571" max="13571" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13572" max="13572" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13573" max="13573" width="8" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13575" max="13575" width="7" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13577" max="13577" width="11.140625" customWidth="1"/>
+    <col min="13578" max="13578" width="2.42578125" customWidth="1"/>
+    <col min="13825" max="13825" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="10.140625" customWidth="1"/>
+    <col min="13827" max="13827" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13828" max="13828" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13829" max="13829" width="8" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13831" max="13831" width="7" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13833" max="13833" width="11.140625" customWidth="1"/>
+    <col min="13834" max="13834" width="2.42578125" customWidth="1"/>
+    <col min="14081" max="14081" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="10.140625" customWidth="1"/>
+    <col min="14083" max="14083" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14084" max="14084" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14085" max="14085" width="8" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14087" max="14087" width="7" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14089" max="14089" width="11.140625" customWidth="1"/>
+    <col min="14090" max="14090" width="2.42578125" customWidth="1"/>
+    <col min="14337" max="14337" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="10.140625" customWidth="1"/>
+    <col min="14339" max="14339" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14340" max="14340" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14341" max="14341" width="8" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14343" max="14343" width="7" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14345" max="14345" width="11.140625" customWidth="1"/>
+    <col min="14346" max="14346" width="2.42578125" customWidth="1"/>
+    <col min="14593" max="14593" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="10.140625" customWidth="1"/>
+    <col min="14595" max="14595" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14596" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14597" max="14597" width="8" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14599" max="14599" width="7" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14601" max="14601" width="11.140625" customWidth="1"/>
+    <col min="14602" max="14602" width="2.42578125" customWidth="1"/>
+    <col min="14849" max="14849" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="10.140625" customWidth="1"/>
+    <col min="14851" max="14851" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14852" max="14852" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14853" max="14853" width="8" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14855" max="14855" width="7" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14857" max="14857" width="11.140625" customWidth="1"/>
+    <col min="14858" max="14858" width="2.42578125" customWidth="1"/>
+    <col min="15105" max="15105" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="10.140625" customWidth="1"/>
+    <col min="15107" max="15107" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15108" max="15108" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15109" max="15109" width="8" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15111" max="15111" width="7" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15113" max="15113" width="11.140625" customWidth="1"/>
+    <col min="15114" max="15114" width="2.42578125" customWidth="1"/>
+    <col min="15361" max="15361" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="10.140625" customWidth="1"/>
+    <col min="15363" max="15363" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15364" max="15364" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15365" max="15365" width="8" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15367" max="15367" width="7" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15369" max="15369" width="11.140625" customWidth="1"/>
+    <col min="15370" max="15370" width="2.42578125" customWidth="1"/>
+    <col min="15617" max="15617" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="10.140625" customWidth="1"/>
+    <col min="15619" max="15619" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15620" max="15620" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15621" max="15621" width="8" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15623" max="15623" width="7" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15625" max="15625" width="11.140625" customWidth="1"/>
+    <col min="15626" max="15626" width="2.42578125" customWidth="1"/>
+    <col min="15873" max="15873" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="10.140625" customWidth="1"/>
+    <col min="15875" max="15875" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15876" max="15876" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15877" max="15877" width="8" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15879" max="15879" width="7" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15881" max="15881" width="11.140625" customWidth="1"/>
+    <col min="15882" max="15882" width="2.42578125" customWidth="1"/>
+    <col min="16129" max="16129" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="10.140625" customWidth="1"/>
+    <col min="16131" max="16131" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16132" max="16132" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16133" width="8" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="7" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16137" max="16137" width="11.140625" customWidth="1"/>
+    <col min="16138" max="16138" width="2.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="26">
+        <v>20634</v>
+      </c>
+      <c r="C5" s="27">
+        <v>52721</v>
+      </c>
+      <c r="D5" s="27">
+        <v>14433</v>
+      </c>
+      <c r="E5" s="27">
+        <v>17953</v>
+      </c>
+      <c r="F5" s="27">
+        <v>8106</v>
+      </c>
+      <c r="G5" s="27">
+        <v>9186</v>
+      </c>
+      <c r="H5" s="27">
+        <v>8680</v>
+      </c>
+      <c r="I5" s="28">
+        <v>131713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="30">
+        <v>24867</v>
+      </c>
+      <c r="C6" s="31">
+        <v>33775</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31">
+        <v>12407</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31">
+        <v>3767</v>
+      </c>
+      <c r="H6" s="31">
+        <v>19929</v>
+      </c>
+      <c r="I6" s="32">
+        <v>94745</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="30">
+        <v>80193</v>
+      </c>
+      <c r="C7" s="31">
+        <v>36094</v>
+      </c>
+      <c r="D7" s="31">
+        <v>680</v>
+      </c>
+      <c r="E7" s="31">
+        <v>5341</v>
+      </c>
+      <c r="F7" s="31">
+        <v>9104</v>
+      </c>
+      <c r="G7" s="31">
+        <v>7388</v>
+      </c>
+      <c r="H7" s="31">
+        <v>2256</v>
+      </c>
+      <c r="I7" s="32">
+        <v>141056</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="30">
+        <v>9082</v>
+      </c>
+      <c r="C8" s="31">
+        <v>39686</v>
+      </c>
+      <c r="D8" s="31">
+        <v>29905</v>
+      </c>
+      <c r="E8" s="31">
+        <v>37197</v>
+      </c>
+      <c r="F8" s="31">
+        <v>21636</v>
+      </c>
+      <c r="G8" s="31">
+        <v>8775</v>
+      </c>
+      <c r="H8" s="31">
+        <v>8887</v>
+      </c>
+      <c r="I8" s="32">
+        <v>155168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="30">
+        <v>10332</v>
+      </c>
+      <c r="C9" s="31">
+        <v>40050</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31">
+        <v>4390</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31">
+        <v>12010</v>
+      </c>
+      <c r="I9" s="32">
+        <v>66782</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="30">
+        <v>17534</v>
+      </c>
+      <c r="C10" s="31">
+        <v>42908</v>
+      </c>
+      <c r="D10" s="31">
+        <v>5100</v>
+      </c>
+      <c r="E10" s="31">
+        <v>38436</v>
+      </c>
+      <c r="F10" s="31">
+        <v>41815</v>
+      </c>
+      <c r="G10" s="31">
+        <v>5600</v>
+      </c>
+      <c r="H10" s="31">
+        <v>21744</v>
+      </c>
+      <c r="I10" s="32">
+        <v>173137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="30">
+        <v>28615</v>
+      </c>
+      <c r="C11" s="31">
+        <v>95061</v>
+      </c>
+      <c r="D11" s="31">
+        <v>7163</v>
+      </c>
+      <c r="E11" s="31">
+        <v>26715</v>
+      </c>
+      <c r="F11" s="31">
+        <v>56284</v>
+      </c>
+      <c r="G11" s="31">
+        <v>22363</v>
+      </c>
+      <c r="H11" s="31">
+        <v>30932</v>
+      </c>
+      <c r="I11" s="32">
+        <v>267133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="34">
+        <v>191257</v>
+      </c>
+      <c r="C12" s="35">
+        <v>340295</v>
+      </c>
+      <c r="D12" s="35">
+        <v>57281</v>
+      </c>
+      <c r="E12" s="35">
+        <v>142439</v>
+      </c>
+      <c r="F12" s="35">
+        <v>136945</v>
+      </c>
+      <c r="G12" s="35">
+        <v>57079</v>
+      </c>
+      <c r="H12" s="35">
+        <v>104438</v>
+      </c>
+      <c r="I12" s="36">
+        <v>1029734</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>